<commit_message>
Slice coding PR.specialty 10254179641be6e64eb225fdf131f1aa0163ee00
</commit_message>
<xml_diff>
--- a/lien-specialty-slice-coding/ig/StructureDefinition-ror-practitionerrole.xlsx
+++ b/lien-specialty-slice-coding/ig/StructureDefinition-ror-practitionerrole.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$83</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2879" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3024" uniqueCount="522">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-13T15:20:10+00:00</t>
+    <t>2024-03-14T16:30:20+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1004,7 +1004,37 @@
     <t>./Specialty</t>
   </si>
   <si>
-    <t>PractitionerRole.specialty:expertiseType</t>
+    <t>PractitionerRole.specialty.id</t>
+  </si>
+  <si>
+    <t>PractitionerRole.specialty.extension</t>
+  </si>
+  <si>
+    <t>PractitionerRole.specialty.coding</t>
+  </si>
+  <si>
+    <t>Code defined by a terminology system</t>
+  </si>
+  <si>
+    <t>A reference to a code defined by a terminology system.</t>
+  </si>
+  <si>
+    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
+  </si>
+  <si>
+    <t>Allows for alternative encodings within a code system, and translations to other code systems.</t>
+  </si>
+  <si>
+    <t>CodeableConcept.coding</t>
+  </si>
+  <si>
+    <t>C*E.1-8, C*E.10-22</t>
+  </si>
+  <si>
+    <t>union(., ./translation)</t>
+  </si>
+  <si>
+    <t>PractitionerRole.specialty.coding:expertiseType</t>
   </si>
   <si>
     <t>expertiseType</t>
@@ -1014,6 +1044,30 @@
   </si>
   <si>
     <t>https://mos.esante.gouv.fr/NOS/JDV_J209-TypeSavoirFaire-ROR/FHIR/JDV-J209-TypeSavoirFaire-ROR</t>
+  </si>
+  <si>
+    <t>PractitionerRole.specialty.text</t>
+  </si>
+  <si>
+    <t>Plain text representation of the concept</t>
+  </si>
+  <si>
+    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
+  </si>
+  <si>
+    <t>Very often the text is the same as a displayName of one of the codings.</t>
+  </si>
+  <si>
+    <t>The codes from the terminologies do not always capture the correct meaning with all the nuances of the human using them, or sometimes there is no appropriate code at all. In these cases, the text is used to capture the full meaning of the source.</t>
+  </si>
+  <si>
+    <t>CodeableConcept.text</t>
+  </si>
+  <si>
+    <t>C*E.9. But note many systems use C*E.2 for this</t>
+  </si>
+  <si>
+    <t>./originalText[mediaType/code="text/plain"]/data</t>
   </si>
   <si>
     <t>PractitionerRole.specialty:specialty</t>
@@ -1902,7 +1956,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN79"/>
+  <dimension ref="A1:AN83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -6071,7 +6125,7 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>78</v>
@@ -6175,42 +6229,38 @@
         <v>316</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="C38" t="s" s="2">
-        <v>317</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
         <v>76</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>87</v>
       </c>
       <c r="H38" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I38" t="s" s="2">
         <v>76</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>228</v>
+        <v>103</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>318</v>
+        <v>104</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>310</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" t="s" s="2">
         <v>76</v>
@@ -6235,11 +6285,13 @@
         <v>76</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="Y38" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="Y38" t="s" s="2">
+        <v>76</v>
+      </c>
       <c r="Z38" t="s" s="2">
-        <v>319</v>
+        <v>76</v>
       </c>
       <c r="AA38" t="s" s="2">
         <v>76</v>
@@ -6257,28 +6309,28 @@
         <v>76</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>307</v>
+        <v>106</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>313</v>
+        <v>76</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>314</v>
+        <v>107</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>315</v>
+        <v>76</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>76</v>
@@ -6286,44 +6338,42 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="C39" t="s" s="2">
-        <v>321</v>
-      </c>
+        <v>317</v>
+      </c>
+      <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
         <v>77</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="H39" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I39" t="s" s="2">
         <v>76</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>228</v>
+        <v>110</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>322</v>
+        <v>111</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>309</v>
+        <v>112</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>310</v>
+        <v>113</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" t="s" s="2">
@@ -6349,29 +6399,31 @@
         <v>76</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="Y39" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="Y39" t="s" s="2">
+        <v>76</v>
+      </c>
       <c r="Z39" t="s" s="2">
-        <v>323</v>
+        <v>76</v>
       </c>
       <c r="AA39" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AB39" t="s" s="2">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="AC39" t="s" s="2">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="AD39" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>307</v>
+        <v>117</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>77</v>
@@ -6383,16 +6435,16 @@
         <v>99</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>313</v>
+        <v>76</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>314</v>
+        <v>101</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>315</v>
+        <v>76</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>76</v>
@@ -6400,26 +6452,24 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="C40" t="s" s="2">
-        <v>325</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
         <v>76</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I40" t="s" s="2">
         <v>76</v>
@@ -6428,18 +6478,20 @@
         <v>88</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>228</v>
+        <v>143</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>309</v>
+        <v>320</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="O40" s="2"/>
+        <v>321</v>
+      </c>
+      <c r="O40" t="s" s="2">
+        <v>322</v>
+      </c>
       <c r="P40" t="s" s="2">
         <v>76</v>
       </c>
@@ -6463,29 +6515,29 @@
         <v>76</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="Y40" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="Y40" t="s" s="2">
+        <v>76</v>
+      </c>
       <c r="Z40" t="s" s="2">
-        <v>327</v>
+        <v>76</v>
       </c>
       <c r="AA40" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AB40" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC40" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="AC40" s="2"/>
       <c r="AD40" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>307</v>
+        <v>323</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>77</v>
@@ -6500,13 +6552,13 @@
         <v>100</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>315</v>
+        <v>76</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>76</v>
@@ -6514,20 +6566,20 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="C41" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D41" t="s" s="2">
         <v>76</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>87</v>
@@ -6542,18 +6594,20 @@
         <v>88</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>228</v>
+        <v>143</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>309</v>
+        <v>320</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="O41" s="2"/>
+        <v>321</v>
+      </c>
+      <c r="O41" t="s" s="2">
+        <v>322</v>
+      </c>
       <c r="P41" t="s" s="2">
         <v>76</v>
       </c>
@@ -6581,7 +6635,7 @@
       </c>
       <c r="Y41" s="2"/>
       <c r="Z41" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="AA41" t="s" s="2">
         <v>76</v>
@@ -6599,7 +6653,7 @@
         <v>76</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>307</v>
+        <v>323</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>77</v>
@@ -6614,13 +6668,13 @@
         <v>100</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>315</v>
+        <v>76</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>76</v>
@@ -6628,14 +6682,12 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="C42" t="s" s="2">
-        <v>333</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
         <v>76</v>
       </c>
@@ -6647,7 +6699,7 @@
         <v>87</v>
       </c>
       <c r="H42" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I42" t="s" s="2">
         <v>76</v>
@@ -6656,18 +6708,20 @@
         <v>88</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>228</v>
+        <v>103</v>
       </c>
       <c r="L42" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="M42" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="N42" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="O42" t="s" s="2">
         <v>334</v>
       </c>
-      <c r="M42" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
         <v>76</v>
       </c>
@@ -6691,35 +6745,37 @@
         <v>76</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="Y42" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="Y42" t="s" s="2">
+        <v>76</v>
+      </c>
       <c r="Z42" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AA42" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB42" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC42" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD42" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE42" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AF42" t="s" s="2">
         <v>335</v>
       </c>
-      <c r="AA42" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB42" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC42" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD42" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE42" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF42" t="s" s="2">
-        <v>307</v>
-      </c>
       <c r="AG42" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AI42" t="s" s="2">
         <v>99</v>
@@ -6728,13 +6784,13 @@
         <v>100</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>313</v>
+        <v>336</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>314</v>
+        <v>337</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>315</v>
+        <v>76</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>76</v>
@@ -6742,13 +6798,13 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B43" t="s" s="2">
         <v>307</v>
       </c>
       <c r="C43" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D43" t="s" s="2">
         <v>76</v>
@@ -6773,7 +6829,7 @@
         <v>228</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="M43" t="s" s="2">
         <v>309</v>
@@ -6809,7 +6865,7 @@
       </c>
       <c r="Y43" s="2"/>
       <c r="Z43" t="s" s="2">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="AA43" t="s" s="2">
         <v>76</v>
@@ -6856,13 +6912,13 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B44" t="s" s="2">
         <v>307</v>
       </c>
       <c r="C44" t="s" s="2">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D44" t="s" s="2">
         <v>76</v>
@@ -6887,7 +6943,7 @@
         <v>228</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="M44" t="s" s="2">
         <v>309</v>
@@ -6923,7 +6979,7 @@
       </c>
       <c r="Y44" s="2"/>
       <c r="Z44" t="s" s="2">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="AA44" t="s" s="2">
         <v>76</v>
@@ -6970,13 +7026,13 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B45" t="s" s="2">
         <v>307</v>
       </c>
       <c r="C45" t="s" s="2">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D45" t="s" s="2">
         <v>76</v>
@@ -7001,7 +7057,7 @@
         <v>228</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="M45" t="s" s="2">
         <v>309</v>
@@ -7037,7 +7093,7 @@
       </c>
       <c r="Y45" s="2"/>
       <c r="Z45" t="s" s="2">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="AA45" t="s" s="2">
         <v>76</v>
@@ -7084,13 +7140,13 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B46" t="s" s="2">
         <v>307</v>
       </c>
       <c r="C46" t="s" s="2">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D46" t="s" s="2">
         <v>76</v>
@@ -7115,7 +7171,7 @@
         <v>228</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="M46" t="s" s="2">
         <v>309</v>
@@ -7151,7 +7207,7 @@
       </c>
       <c r="Y46" s="2"/>
       <c r="Z46" t="s" s="2">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="AA46" t="s" s="2">
         <v>76</v>
@@ -7198,13 +7254,13 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B47" t="s" s="2">
         <v>307</v>
       </c>
       <c r="C47" t="s" s="2">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D47" t="s" s="2">
         <v>76</v>
@@ -7214,7 +7270,7 @@
         <v>77</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="H47" t="s" s="2">
         <v>88</v>
@@ -7229,7 +7285,7 @@
         <v>228</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="M47" t="s" s="2">
         <v>309</v>
@@ -7265,7 +7321,7 @@
       </c>
       <c r="Y47" s="2"/>
       <c r="Z47" t="s" s="2">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="AA47" t="s" s="2">
         <v>76</v>
@@ -7312,12 +7368,14 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="C48" s="2"/>
+        <v>307</v>
+      </c>
+      <c r="C48" t="s" s="2">
+        <v>359</v>
+      </c>
       <c r="D48" t="s" s="2">
         <v>76</v>
       </c>
@@ -7326,10 +7384,10 @@
         <v>77</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I48" t="s" s="2">
         <v>76</v>
@@ -7338,16 +7396,16 @@
         <v>88</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>357</v>
+        <v>228</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>359</v>
+        <v>309</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
@@ -7373,13 +7431,11 @@
         <v>76</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y48" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="Y48" s="2"/>
       <c r="Z48" t="s" s="2">
-        <v>76</v>
+        <v>361</v>
       </c>
       <c r="AA48" t="s" s="2">
         <v>76</v>
@@ -7397,7 +7453,7 @@
         <v>76</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>356</v>
+        <v>307</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>77</v>
@@ -7409,35 +7465,37 @@
         <v>99</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>292</v>
+        <v>100</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>76</v>
+        <v>313</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>360</v>
+        <v>314</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>361</v>
+        <v>315</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>362</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="B49" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="C49" t="s" s="2">
         <v>363</v>
       </c>
-      <c r="B49" t="s" s="2">
-        <v>363</v>
-      </c>
-      <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
         <v>76</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>87</v>
@@ -7449,19 +7507,19 @@
         <v>76</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>364</v>
       </c>
-      <c r="L49" t="s" s="2">
-        <v>365</v>
-      </c>
       <c r="M49" t="s" s="2">
-        <v>366</v>
+        <v>309</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="O49" s="2"/>
       <c r="P49" t="s" s="2">
@@ -7487,13 +7545,11 @@
         <v>76</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y49" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="Y49" s="2"/>
       <c r="Z49" t="s" s="2">
-        <v>76</v>
+        <v>365</v>
       </c>
       <c r="AA49" t="s" s="2">
         <v>76</v>
@@ -7511,7 +7567,7 @@
         <v>76</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>363</v>
+        <v>307</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>77</v>
@@ -7523,16 +7579,16 @@
         <v>99</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>292</v>
+        <v>100</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>367</v>
+        <v>313</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>368</v>
+        <v>314</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>76</v>
+        <v>315</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>76</v>
@@ -7540,12 +7596,14 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>369</v>
-      </c>
-      <c r="C50" s="2"/>
+        <v>307</v>
+      </c>
+      <c r="C50" t="s" s="2">
+        <v>367</v>
+      </c>
       <c r="D50" t="s" s="2">
         <v>76</v>
       </c>
@@ -7566,18 +7624,18 @@
         <v>88</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>370</v>
+        <v>228</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>372</v>
-      </c>
-      <c r="N50" s="2"/>
-      <c r="O50" t="s" s="2">
-        <v>373</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="N50" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
         <v>76</v>
       </c>
@@ -7601,13 +7659,11 @@
         <v>76</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y50" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="Y50" s="2"/>
       <c r="Z50" t="s" s="2">
-        <v>76</v>
+        <v>369</v>
       </c>
       <c r="AA50" t="s" s="2">
         <v>76</v>
@@ -7625,7 +7681,7 @@
         <v>76</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>369</v>
+        <v>307</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>77</v>
@@ -7637,16 +7693,16 @@
         <v>99</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>374</v>
+        <v>100</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>375</v>
+        <v>313</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>376</v>
+        <v>314</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>377</v>
+        <v>315</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>76</v>
@@ -7654,12 +7710,14 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>378</v>
-      </c>
-      <c r="C51" s="2"/>
+        <v>307</v>
+      </c>
+      <c r="C51" t="s" s="2">
+        <v>371</v>
+      </c>
       <c r="D51" t="s" s="2">
         <v>76</v>
       </c>
@@ -7668,27 +7726,29 @@
         <v>77</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="H51" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I51" t="s" s="2">
         <v>76</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>103</v>
+        <v>228</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>104</v>
+        <v>372</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="N51" s="2"/>
+        <v>309</v>
+      </c>
+      <c r="N51" t="s" s="2">
+        <v>310</v>
+      </c>
       <c r="O51" s="2"/>
       <c r="P51" t="s" s="2">
         <v>76</v>
@@ -7713,13 +7773,11 @@
         <v>76</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y51" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="Y51" s="2"/>
       <c r="Z51" t="s" s="2">
-        <v>76</v>
+        <v>373</v>
       </c>
       <c r="AA51" t="s" s="2">
         <v>76</v>
@@ -7737,28 +7795,28 @@
         <v>76</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>106</v>
+        <v>307</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>76</v>
+        <v>313</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>107</v>
+        <v>314</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>76</v>
+        <v>315</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>76</v>
@@ -7766,10 +7824,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7777,7 +7835,7 @@
       </c>
       <c r="E52" s="2"/>
       <c r="F52" t="s" s="2">
-        <v>196</v>
+        <v>77</v>
       </c>
       <c r="G52" t="s" s="2">
         <v>78</v>
@@ -7789,18 +7847,20 @@
         <v>76</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>110</v>
+        <v>375</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>197</v>
+        <v>376</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="N52" s="2"/>
+        <v>377</v>
+      </c>
+      <c r="N52" t="s" s="2">
+        <v>291</v>
+      </c>
       <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
         <v>76</v>
@@ -7837,19 +7897,19 @@
         <v>76</v>
       </c>
       <c r="AB52" t="s" s="2">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="AC52" t="s" s="2">
-        <v>115</v>
+        <v>76</v>
       </c>
       <c r="AD52" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>117</v>
+        <v>374</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>77</v>
@@ -7861,31 +7921,29 @@
         <v>99</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>118</v>
+        <v>292</v>
       </c>
       <c r="AK52" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>76</v>
+        <v>378</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>76</v>
+        <v>379</v>
       </c>
       <c r="AN52" t="s" s="2">
-        <v>76</v>
+        <v>380</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>379</v>
-      </c>
-      <c r="C53" t="s" s="2">
         <v>381</v>
       </c>
+      <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
         <v>76</v>
       </c>
@@ -7914,7 +7972,9 @@
       <c r="M53" t="s" s="2">
         <v>384</v>
       </c>
-      <c r="N53" s="2"/>
+      <c r="N53" t="s" s="2">
+        <v>291</v>
+      </c>
       <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
         <v>76</v>
@@ -7963,7 +8023,7 @@
         <v>76</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>117</v>
+        <v>381</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>77</v>
@@ -7975,13 +8035,13 @@
         <v>99</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>118</v>
+        <v>292</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>76</v>
+        <v>385</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>76</v>
+        <v>386</v>
       </c>
       <c r="AM53" t="s" s="2">
         <v>76</v>
@@ -7992,14 +8052,12 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>379</v>
-      </c>
-      <c r="C54" t="s" s="2">
-        <v>386</v>
-      </c>
+        <v>387</v>
+      </c>
+      <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
         <v>76</v>
       </c>
@@ -8017,19 +8075,21 @@
         <v>76</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="N54" s="2"/>
-      <c r="O54" s="2"/>
+      <c r="O54" t="s" s="2">
+        <v>391</v>
+      </c>
       <c r="P54" t="s" s="2">
         <v>76</v>
       </c>
@@ -8077,7 +8137,7 @@
         <v>76</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>117</v>
+        <v>387</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>77</v>
@@ -8089,16 +8149,16 @@
         <v>99</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>118</v>
+        <v>392</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>76</v>
+        <v>393</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>76</v>
+        <v>394</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>76</v>
+        <v>395</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>76</v>
@@ -8106,26 +8166,24 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>379</v>
-      </c>
-      <c r="C55" t="s" s="2">
-        <v>391</v>
-      </c>
+        <v>396</v>
+      </c>
+      <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
         <v>76</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G55" t="s" s="2">
         <v>87</v>
       </c>
       <c r="H55" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I55" t="s" s="2">
         <v>76</v>
@@ -8134,13 +8192,13 @@
         <v>76</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>392</v>
+        <v>103</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>393</v>
+        <v>104</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>394</v>
+        <v>105</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -8191,25 +8249,25 @@
         <v>76</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH55" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="AM55" t="s" s="2">
         <v>76</v>
@@ -8220,10 +8278,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8231,10 +8289,10 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s" s="2">
-        <v>77</v>
+        <v>196</v>
       </c>
       <c r="G56" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="H56" t="s" s="2">
         <v>76</v>
@@ -8243,20 +8301,18 @@
         <v>76</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>172</v>
+        <v>110</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>396</v>
+        <v>197</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>397</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>398</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="N56" s="2"/>
       <c r="O56" s="2"/>
       <c r="P56" t="s" s="2">
         <v>76</v>
@@ -8281,52 +8337,52 @@
         <v>76</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>164</v>
+        <v>76</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>399</v>
+        <v>76</v>
       </c>
       <c r="Z56" t="s" s="2">
-        <v>400</v>
+        <v>76</v>
       </c>
       <c r="AA56" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AB56" t="s" s="2">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="AC56" t="s" s="2">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="AD56" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>401</v>
+        <v>117</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH56" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>402</v>
+        <v>99</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>403</v>
+        <v>76</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>404</v>
+        <v>76</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>405</v>
+        <v>76</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>76</v>
@@ -8334,12 +8390,14 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>406</v>
-      </c>
-      <c r="C57" s="2"/>
+        <v>397</v>
+      </c>
+      <c r="C57" t="s" s="2">
+        <v>399</v>
+      </c>
       <c r="D57" t="s" s="2">
         <v>76</v>
       </c>
@@ -8357,23 +8415,19 @@
         <v>76</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>103</v>
+        <v>400</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>408</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>409</v>
-      </c>
-      <c r="O57" t="s" s="2">
-        <v>410</v>
-      </c>
+        <v>402</v>
+      </c>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
       <c r="P57" t="s" s="2">
         <v>76</v>
       </c>
@@ -8421,28 +8475,28 @@
         <v>76</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>411</v>
+        <v>117</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH57" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AI57" t="s" s="2">
         <v>99</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>412</v>
+        <v>76</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>413</v>
+        <v>76</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>414</v>
+        <v>76</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>76</v>
@@ -8450,12 +8504,14 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>415</v>
-      </c>
-      <c r="C58" s="2"/>
+        <v>397</v>
+      </c>
+      <c r="C58" t="s" s="2">
+        <v>404</v>
+      </c>
       <c r="D58" t="s" s="2">
         <v>76</v>
       </c>
@@ -8467,29 +8523,25 @@
         <v>87</v>
       </c>
       <c r="H58" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>172</v>
+        <v>405</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>417</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>418</v>
-      </c>
-      <c r="O58" t="s" s="2">
-        <v>419</v>
-      </c>
+        <v>407</v>
+      </c>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
       <c r="P58" t="s" s="2">
         <v>76</v>
       </c>
@@ -8513,13 +8565,13 @@
         <v>76</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>164</v>
+        <v>76</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>420</v>
+        <v>76</v>
       </c>
       <c r="Z58" t="s" s="2">
-        <v>421</v>
+        <v>76</v>
       </c>
       <c r="AA58" t="s" s="2">
         <v>76</v>
@@ -8537,28 +8589,28 @@
         <v>76</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>422</v>
+        <v>117</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH58" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AI58" t="s" s="2">
         <v>99</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>423</v>
+        <v>76</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>424</v>
+        <v>76</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>425</v>
+        <v>76</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>76</v>
@@ -8566,43 +8618,43 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>426</v>
-      </c>
-      <c r="C59" s="2"/>
+        <v>397</v>
+      </c>
+      <c r="C59" t="s" s="2">
+        <v>409</v>
+      </c>
       <c r="D59" t="s" s="2">
         <v>76</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G59" t="s" s="2">
         <v>87</v>
       </c>
       <c r="H59" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I59" t="s" s="2">
         <v>76</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>429</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>430</v>
-      </c>
+        <v>412</v>
+      </c>
+      <c r="N59" s="2"/>
       <c r="O59" s="2"/>
       <c r="P59" t="s" s="2">
         <v>76</v>
@@ -8651,25 +8703,25 @@
         <v>76</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>431</v>
+        <v>117</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>99</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="AM59" t="s" s="2">
         <v>76</v>
@@ -8680,10 +8732,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>432</v>
+        <v>413</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>432</v>
+        <v>413</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8706,16 +8758,16 @@
         <v>88</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>277</v>
+        <v>172</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>433</v>
+        <v>414</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>434</v>
+        <v>415</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>280</v>
+        <v>416</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
@@ -8741,13 +8793,13 @@
         <v>76</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>76</v>
+        <v>164</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>76</v>
+        <v>417</v>
       </c>
       <c r="Z60" t="s" s="2">
-        <v>76</v>
+        <v>418</v>
       </c>
       <c r="AA60" t="s" s="2">
         <v>76</v>
@@ -8765,7 +8817,7 @@
         <v>76</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>435</v>
+        <v>419</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>77</v>
@@ -8774,19 +8826,19 @@
         <v>87</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>99</v>
+        <v>420</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>282</v>
+        <v>100</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>101</v>
+        <v>421</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>437</v>
+        <v>423</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>76</v>
@@ -8794,10 +8846,10 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -8805,7 +8857,7 @@
       </c>
       <c r="E61" s="2"/>
       <c r="F61" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G61" t="s" s="2">
         <v>87</v>
@@ -8817,21 +8869,23 @@
         <v>76</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>439</v>
+        <v>103</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>441</v>
+        <v>426</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>442</v>
-      </c>
-      <c r="O61" s="2"/>
+        <v>427</v>
+      </c>
+      <c r="O61" t="s" s="2">
+        <v>428</v>
+      </c>
       <c r="P61" t="s" s="2">
         <v>76</v>
       </c>
@@ -8879,13 +8933,13 @@
         <v>76</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH61" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AI61" t="s" s="2">
         <v>99</v>
@@ -8894,13 +8948,13 @@
         <v>100</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>76</v>
+        <v>430</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>76</v>
+        <v>432</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>76</v>
@@ -8908,10 +8962,10 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -8928,22 +8982,26 @@
         <v>76</v>
       </c>
       <c r="I62" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>103</v>
+        <v>172</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>104</v>
+        <v>434</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="N62" s="2"/>
-      <c r="O62" s="2"/>
+        <v>435</v>
+      </c>
+      <c r="N62" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="O62" t="s" s="2">
+        <v>437</v>
+      </c>
       <c r="P62" t="s" s="2">
         <v>76</v>
       </c>
@@ -8967,13 +9025,13 @@
         <v>76</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>76</v>
+        <v>164</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>76</v>
+        <v>438</v>
       </c>
       <c r="Z62" t="s" s="2">
-        <v>76</v>
+        <v>439</v>
       </c>
       <c r="AA62" t="s" s="2">
         <v>76</v>
@@ -8991,7 +9049,7 @@
         <v>76</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>106</v>
+        <v>440</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>77</v>
@@ -9000,19 +9058,19 @@
         <v>87</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>76</v>
+        <v>441</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>107</v>
+        <v>442</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>76</v>
+        <v>443</v>
       </c>
       <c r="AN62" t="s" s="2">
         <v>76</v>
@@ -9020,21 +9078,21 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" t="s" s="2">
         <v>77</v>
       </c>
       <c r="G63" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="H63" t="s" s="2">
         <v>76</v>
@@ -9043,19 +9101,19 @@
         <v>76</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>110</v>
+        <v>445</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>111</v>
+        <v>446</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>112</v>
+        <v>447</v>
       </c>
       <c r="N63" t="s" s="2">
-        <v>113</v>
+        <v>448</v>
       </c>
       <c r="O63" s="2"/>
       <c r="P63" t="s" s="2">
@@ -9093,37 +9151,37 @@
         <v>76</v>
       </c>
       <c r="AB63" t="s" s="2">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="AC63" t="s" s="2">
-        <v>115</v>
+        <v>76</v>
       </c>
       <c r="AD63" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>117</v>
+        <v>449</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH63" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AI63" t="s" s="2">
         <v>99</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="AM63" t="s" s="2">
         <v>76</v>
@@ -9134,14 +9192,12 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>445</v>
-      </c>
-      <c r="C64" t="s" s="2">
-        <v>447</v>
-      </c>
+        <v>450</v>
+      </c>
+      <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
         <v>76</v>
       </c>
@@ -9153,24 +9209,26 @@
         <v>87</v>
       </c>
       <c r="H64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J64" t="s" s="2">
         <v>88</v>
       </c>
-      <c r="I64" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J64" t="s" s="2">
-        <v>76</v>
-      </c>
       <c r="K64" t="s" s="2">
-        <v>448</v>
+        <v>277</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>450</v>
-      </c>
-      <c r="N64" s="2"/>
+        <v>452</v>
+      </c>
+      <c r="N64" t="s" s="2">
+        <v>280</v>
+      </c>
       <c r="O64" s="2"/>
       <c r="P64" t="s" s="2">
         <v>76</v>
@@ -9219,28 +9277,28 @@
         <v>76</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>117</v>
+        <v>453</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH64" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AI64" t="s" s="2">
         <v>99</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>118</v>
+        <v>282</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>76</v>
+        <v>454</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>76</v>
+        <v>455</v>
       </c>
       <c r="AN64" t="s" s="2">
         <v>76</v>
@@ -9248,14 +9306,12 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>445</v>
-      </c>
-      <c r="C65" t="s" s="2">
-        <v>452</v>
-      </c>
+        <v>456</v>
+      </c>
+      <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
         <v>76</v>
       </c>
@@ -9276,15 +9332,17 @@
         <v>76</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>455</v>
-      </c>
-      <c r="N65" s="2"/>
+        <v>459</v>
+      </c>
+      <c r="N65" t="s" s="2">
+        <v>460</v>
+      </c>
       <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
         <v>76</v>
@@ -9333,7 +9391,7 @@
         <v>76</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>117</v>
+        <v>456</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>77</v>
@@ -9345,13 +9403,13 @@
         <v>99</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="AK65" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>76</v>
+        <v>461</v>
       </c>
       <c r="AM65" t="s" s="2">
         <v>76</v>
@@ -9362,14 +9420,12 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>445</v>
-      </c>
-      <c r="C66" t="s" s="2">
-        <v>457</v>
-      </c>
+        <v>462</v>
+      </c>
+      <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
         <v>76</v>
       </c>
@@ -9381,7 +9437,7 @@
         <v>87</v>
       </c>
       <c r="H66" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I66" t="s" s="2">
         <v>76</v>
@@ -9390,13 +9446,13 @@
         <v>76</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>458</v>
+        <v>103</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>459</v>
+        <v>104</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>460</v>
+        <v>105</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
@@ -9447,25 +9503,25 @@
         <v>76</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH66" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AI66" t="s" s="2">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="AJ66" t="s" s="2">
-        <v>118</v>
+        <v>76</v>
       </c>
       <c r="AK66" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="AM66" t="s" s="2">
         <v>76</v>
@@ -9476,14 +9532,14 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
-        <v>462</v>
+        <v>109</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" t="s" s="2">
@@ -9496,26 +9552,24 @@
         <v>76</v>
       </c>
       <c r="I67" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="K67" t="s" s="2">
         <v>110</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>463</v>
+        <v>111</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>464</v>
+        <v>112</v>
       </c>
       <c r="N67" t="s" s="2">
         <v>113</v>
       </c>
-      <c r="O67" t="s" s="2">
-        <v>255</v>
-      </c>
+      <c r="O67" s="2"/>
       <c r="P67" t="s" s="2">
         <v>76</v>
       </c>
@@ -9551,19 +9605,19 @@
         <v>76</v>
       </c>
       <c r="AB67" t="s" s="2">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="AC67" t="s" s="2">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="AD67" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>465</v>
+        <v>117</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>77</v>
@@ -9592,12 +9646,14 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>466</v>
-      </c>
-      <c r="C68" s="2"/>
+        <v>463</v>
+      </c>
+      <c r="C68" t="s" s="2">
+        <v>465</v>
+      </c>
       <c r="D68" t="s" s="2">
         <v>76</v>
       </c>
@@ -9606,10 +9662,10 @@
         <v>77</v>
       </c>
       <c r="G68" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="H68" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I68" t="s" s="2">
         <v>76</v>
@@ -9618,7 +9674,7 @@
         <v>76</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>172</v>
+        <v>466</v>
       </c>
       <c r="L68" t="s" s="2">
         <v>467</v>
@@ -9626,9 +9682,7 @@
       <c r="M68" t="s" s="2">
         <v>468</v>
       </c>
-      <c r="N68" t="s" s="2">
-        <v>398</v>
-      </c>
+      <c r="N68" s="2"/>
       <c r="O68" s="2"/>
       <c r="P68" t="s" s="2">
         <v>76</v>
@@ -9653,13 +9707,13 @@
         <v>76</v>
       </c>
       <c r="X68" t="s" s="2">
-        <v>164</v>
+        <v>76</v>
       </c>
       <c r="Y68" t="s" s="2">
-        <v>469</v>
+        <v>76</v>
       </c>
       <c r="Z68" t="s" s="2">
-        <v>470</v>
+        <v>76</v>
       </c>
       <c r="AA68" t="s" s="2">
         <v>76</v>
@@ -9677,7 +9731,7 @@
         <v>76</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>466</v>
+        <v>117</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>77</v>
@@ -9689,13 +9743,13 @@
         <v>99</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="AK68" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>443</v>
+        <v>76</v>
       </c>
       <c r="AM68" t="s" s="2">
         <v>76</v>
@@ -9706,12 +9760,14 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>471</v>
-      </c>
-      <c r="C69" s="2"/>
+        <v>463</v>
+      </c>
+      <c r="C69" t="s" s="2">
+        <v>470</v>
+      </c>
       <c r="D69" t="s" s="2">
         <v>76</v>
       </c>
@@ -9723,7 +9779,7 @@
         <v>87</v>
       </c>
       <c r="H69" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I69" t="s" s="2">
         <v>76</v>
@@ -9732,7 +9788,7 @@
         <v>76</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>267</v>
+        <v>471</v>
       </c>
       <c r="L69" t="s" s="2">
         <v>472</v>
@@ -9789,25 +9845,25 @@
         <v>76</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>471</v>
+        <v>117</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AI69" t="s" s="2">
         <v>99</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="AK69" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>443</v>
+        <v>76</v>
       </c>
       <c r="AM69" t="s" s="2">
         <v>76</v>
@@ -9821,9 +9877,11 @@
         <v>474</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>474</v>
-      </c>
-      <c r="C70" s="2"/>
+        <v>463</v>
+      </c>
+      <c r="C70" t="s" s="2">
+        <v>475</v>
+      </c>
       <c r="D70" t="s" s="2">
         <v>76</v>
       </c>
@@ -9844,17 +9902,15 @@
         <v>76</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>477</v>
-      </c>
-      <c r="N70" t="s" s="2">
         <v>478</v>
       </c>
+      <c r="N70" s="2"/>
       <c r="O70" s="2"/>
       <c r="P70" t="s" s="2">
         <v>76</v>
@@ -9903,25 +9959,25 @@
         <v>76</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>474</v>
+        <v>117</v>
       </c>
       <c r="AG70" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH70" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AI70" t="s" s="2">
         <v>99</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="AK70" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>443</v>
+        <v>76</v>
       </c>
       <c r="AM70" t="s" s="2">
         <v>76</v>
@@ -9939,37 +9995,39 @@
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
-        <v>76</v>
+        <v>480</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" t="s" s="2">
         <v>77</v>
       </c>
       <c r="G71" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="H71" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I71" t="s" s="2">
         <v>88</v>
       </c>
-      <c r="I71" t="s" s="2">
-        <v>76</v>
-      </c>
       <c r="J71" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>475</v>
+        <v>110</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="N71" t="s" s="2">
-        <v>478</v>
-      </c>
-      <c r="O71" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="O71" t="s" s="2">
+        <v>255</v>
+      </c>
       <c r="P71" t="s" s="2">
         <v>76</v>
       </c>
@@ -10017,25 +10075,25 @@
         <v>76</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH71" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AI71" t="s" s="2">
         <v>99</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="AK71" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL71" t="s" s="2">
-        <v>443</v>
+        <v>101</v>
       </c>
       <c r="AM71" t="s" s="2">
         <v>76</v>
@@ -10046,10 +10104,10 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10072,15 +10130,17 @@
         <v>76</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>439</v>
+        <v>172</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>484</v>
-      </c>
-      <c r="N72" s="2"/>
+        <v>486</v>
+      </c>
+      <c r="N72" t="s" s="2">
+        <v>416</v>
+      </c>
       <c r="O72" s="2"/>
       <c r="P72" t="s" s="2">
         <v>76</v>
@@ -10105,13 +10165,13 @@
         <v>76</v>
       </c>
       <c r="X72" t="s" s="2">
-        <v>76</v>
+        <v>164</v>
       </c>
       <c r="Y72" t="s" s="2">
-        <v>76</v>
+        <v>487</v>
       </c>
       <c r="Z72" t="s" s="2">
-        <v>76</v>
+        <v>488</v>
       </c>
       <c r="AA72" t="s" s="2">
         <v>76</v>
@@ -10129,7 +10189,7 @@
         <v>76</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>77</v>
@@ -10147,7 +10207,7 @@
         <v>76</v>
       </c>
       <c r="AL72" t="s" s="2">
-        <v>443</v>
+        <v>461</v>
       </c>
       <c r="AM72" t="s" s="2">
         <v>76</v>
@@ -10158,10 +10218,10 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10184,13 +10244,13 @@
         <v>76</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>103</v>
+        <v>267</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>104</v>
+        <v>490</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>105</v>
+        <v>491</v>
       </c>
       <c r="N73" s="2"/>
       <c r="O73" s="2"/>
@@ -10241,7 +10301,7 @@
         <v>76</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>106</v>
+        <v>489</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>77</v>
@@ -10250,16 +10310,16 @@
         <v>87</v>
       </c>
       <c r="AI73" t="s" s="2">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="AJ73" t="s" s="2">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="AK73" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>107</v>
+        <v>461</v>
       </c>
       <c r="AM73" t="s" s="2">
         <v>76</v>
@@ -10270,24 +10330,24 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" t="s" s="2">
         <v>77</v>
       </c>
       <c r="G74" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="H74" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I74" t="s" s="2">
         <v>76</v>
@@ -10296,16 +10356,16 @@
         <v>76</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>110</v>
+        <v>493</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>111</v>
+        <v>494</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>112</v>
+        <v>495</v>
       </c>
       <c r="N74" t="s" s="2">
-        <v>113</v>
+        <v>496</v>
       </c>
       <c r="O74" s="2"/>
       <c r="P74" t="s" s="2">
@@ -10343,37 +10403,37 @@
         <v>76</v>
       </c>
       <c r="AB74" t="s" s="2">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="AC74" t="s" s="2">
-        <v>115</v>
+        <v>76</v>
       </c>
       <c r="AD74" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>117</v>
+        <v>492</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH74" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AI74" t="s" s="2">
         <v>99</v>
       </c>
       <c r="AJ74" t="s" s="2">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="AK74" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL74" t="s" s="2">
-        <v>101</v>
+        <v>461</v>
       </c>
       <c r="AM74" t="s" s="2">
         <v>76</v>
@@ -10384,46 +10444,44 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>487</v>
+        <v>497</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>487</v>
+        <v>497</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
-        <v>462</v>
+        <v>76</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" t="s" s="2">
         <v>77</v>
       </c>
       <c r="G75" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="H75" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I75" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>110</v>
+        <v>493</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>463</v>
+        <v>498</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>464</v>
+        <v>499</v>
       </c>
       <c r="N75" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="O75" t="s" s="2">
-        <v>255</v>
-      </c>
+        <v>496</v>
+      </c>
+      <c r="O75" s="2"/>
       <c r="P75" t="s" s="2">
         <v>76</v>
       </c>
@@ -10471,25 +10529,25 @@
         <v>76</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>465</v>
+        <v>497</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH75" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="AI75" t="s" s="2">
         <v>99</v>
       </c>
       <c r="AJ75" t="s" s="2">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="AK75" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL75" t="s" s="2">
-        <v>101</v>
+        <v>461</v>
       </c>
       <c r="AM75" t="s" s="2">
         <v>76</v>
@@ -10500,10 +10558,10 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>488</v>
+        <v>500</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>488</v>
+        <v>500</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
@@ -10511,10 +10569,10 @@
       </c>
       <c r="E76" s="2"/>
       <c r="F76" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G76" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="H76" t="s" s="2">
         <v>76</v>
@@ -10526,17 +10584,15 @@
         <v>76</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>103</v>
+        <v>457</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>489</v>
+        <v>501</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>490</v>
-      </c>
-      <c r="N76" t="s" s="2">
-        <v>398</v>
-      </c>
+        <v>502</v>
+      </c>
+      <c r="N76" s="2"/>
       <c r="O76" s="2"/>
       <c r="P76" t="s" s="2">
         <v>76</v>
@@ -10585,13 +10641,13 @@
         <v>76</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>488</v>
+        <v>500</v>
       </c>
       <c r="AG76" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="AH76" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AI76" t="s" s="2">
         <v>99</v>
@@ -10603,7 +10659,7 @@
         <v>76</v>
       </c>
       <c r="AL76" t="s" s="2">
-        <v>107</v>
+        <v>461</v>
       </c>
       <c r="AM76" t="s" s="2">
         <v>76</v>
@@ -10614,10 +10670,10 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>491</v>
+        <v>503</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>491</v>
+        <v>503</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -10640,17 +10696,15 @@
         <v>76</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>277</v>
+        <v>103</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>492</v>
+        <v>104</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>493</v>
-      </c>
-      <c r="N77" t="s" s="2">
-        <v>280</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="N77" s="2"/>
       <c r="O77" s="2"/>
       <c r="P77" t="s" s="2">
         <v>76</v>
@@ -10699,7 +10753,7 @@
         <v>76</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>491</v>
+        <v>106</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>77</v>
@@ -10708,16 +10762,16 @@
         <v>87</v>
       </c>
       <c r="AI77" t="s" s="2">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>282</v>
+        <v>76</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>494</v>
+        <v>76</v>
       </c>
       <c r="AL77" t="s" s="2">
-        <v>443</v>
+        <v>107</v>
       </c>
       <c r="AM77" t="s" s="2">
         <v>76</v>
@@ -10728,21 +10782,21 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>495</v>
+        <v>504</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>495</v>
+        <v>504</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" t="s" s="2">
         <v>77</v>
       </c>
       <c r="G78" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="H78" t="s" s="2">
         <v>76</v>
@@ -10754,16 +10808,16 @@
         <v>76</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>496</v>
+        <v>111</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>497</v>
+        <v>112</v>
       </c>
       <c r="N78" t="s" s="2">
-        <v>398</v>
+        <v>113</v>
       </c>
       <c r="O78" s="2"/>
       <c r="P78" t="s" s="2">
@@ -10801,37 +10855,37 @@
         <v>76</v>
       </c>
       <c r="AB78" t="s" s="2">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="AC78" t="s" s="2">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="AD78" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>495</v>
+        <v>117</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AH78" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="AI78" t="s" s="2">
         <v>99</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="AK78" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL78" t="s" s="2">
-        <v>443</v>
+        <v>101</v>
       </c>
       <c r="AM78" t="s" s="2">
         <v>76</v>
@@ -10842,14 +10896,14 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
-        <v>76</v>
+        <v>480</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" t="s" s="2">
@@ -10862,25 +10916,25 @@
         <v>76</v>
       </c>
       <c r="I79" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="J79" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>499</v>
+        <v>110</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>500</v>
+        <v>481</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>501</v>
+        <v>482</v>
       </c>
       <c r="N79" t="s" s="2">
-        <v>291</v>
+        <v>113</v>
       </c>
       <c r="O79" t="s" s="2">
-        <v>502</v>
+        <v>255</v>
       </c>
       <c r="P79" t="s" s="2">
         <v>76</v>
@@ -10929,7 +10983,7 @@
         <v>76</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>498</v>
+        <v>483</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>77</v>
@@ -10941,23 +10995,481 @@
         <v>99</v>
       </c>
       <c r="AJ79" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="AK79" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL79" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="AM79" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AN79" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="80" hidden="true">
+      <c r="A80" t="s" s="2">
+        <v>506</v>
+      </c>
+      <c r="B80" t="s" s="2">
+        <v>506</v>
+      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="E80" s="2"/>
+      <c r="F80" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="G80" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="K80" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="L80" t="s" s="2">
+        <v>507</v>
+      </c>
+      <c r="M80" t="s" s="2">
+        <v>508</v>
+      </c>
+      <c r="N80" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="O80" s="2"/>
+      <c r="P80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Q80" s="2"/>
+      <c r="R80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="S80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="T80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="U80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="V80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="W80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="X80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Y80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Z80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AA80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AF80" t="s" s="2">
+        <v>506</v>
+      </c>
+      <c r="AG80" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AH80" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI80" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AJ80" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AK80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL80" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="AM80" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AN80" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" hidden="true">
+      <c r="A81" t="s" s="2">
+        <v>509</v>
+      </c>
+      <c r="B81" t="s" s="2">
+        <v>509</v>
+      </c>
+      <c r="C81" s="2"/>
+      <c r="D81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="E81" s="2"/>
+      <c r="F81" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="G81" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="K81" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="L81" t="s" s="2">
+        <v>510</v>
+      </c>
+      <c r="M81" t="s" s="2">
+        <v>511</v>
+      </c>
+      <c r="N81" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="O81" s="2"/>
+      <c r="P81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Q81" s="2"/>
+      <c r="R81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="S81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="T81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="U81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="V81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="W81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="X81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Y81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Z81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AA81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AF81" t="s" s="2">
+        <v>509</v>
+      </c>
+      <c r="AG81" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AH81" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI81" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AJ81" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="AK81" t="s" s="2">
+        <v>512</v>
+      </c>
+      <c r="AL81" t="s" s="2">
+        <v>461</v>
+      </c>
+      <c r="AM81" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AN81" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" hidden="true">
+      <c r="A82" t="s" s="2">
+        <v>513</v>
+      </c>
+      <c r="B82" t="s" s="2">
+        <v>513</v>
+      </c>
+      <c r="C82" s="2"/>
+      <c r="D82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="E82" s="2"/>
+      <c r="F82" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="G82" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="K82" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="L82" t="s" s="2">
+        <v>514</v>
+      </c>
+      <c r="M82" t="s" s="2">
+        <v>515</v>
+      </c>
+      <c r="N82" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="O82" s="2"/>
+      <c r="P82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Q82" s="2"/>
+      <c r="R82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="S82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="T82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="U82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="V82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="W82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="X82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Y82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Z82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AA82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AF82" t="s" s="2">
+        <v>513</v>
+      </c>
+      <c r="AG82" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AH82" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI82" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AJ82" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AK82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL82" t="s" s="2">
+        <v>461</v>
+      </c>
+      <c r="AM82" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AN82" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="83" hidden="true">
+      <c r="A83" t="s" s="2">
+        <v>516</v>
+      </c>
+      <c r="B83" t="s" s="2">
+        <v>516</v>
+      </c>
+      <c r="C83" s="2"/>
+      <c r="D83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="E83" s="2"/>
+      <c r="F83" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="G83" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="H83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="K83" t="s" s="2">
+        <v>517</v>
+      </c>
+      <c r="L83" t="s" s="2">
+        <v>518</v>
+      </c>
+      <c r="M83" t="s" s="2">
+        <v>519</v>
+      </c>
+      <c r="N83" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="O83" t="s" s="2">
+        <v>520</v>
+      </c>
+      <c r="P83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Q83" s="2"/>
+      <c r="R83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="S83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="T83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="U83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="V83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="W83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="X83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Y83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Z83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AA83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AF83" t="s" s="2">
+        <v>516</v>
+      </c>
+      <c r="AG83" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AH83" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AI83" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AJ83" t="s" s="2">
         <v>292</v>
       </c>
-      <c r="AK79" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL79" t="s" s="2">
-        <v>503</v>
-      </c>
-      <c r="AM79" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN79" t="s" s="2">
+      <c r="AK83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL83" t="s" s="2">
+        <v>521</v>
+      </c>
+      <c r="AM83" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AN83" t="s" s="2">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN79">
+  <autoFilter ref="A1:AN83">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10967,7 +11479,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI78">
+  <conditionalFormatting sqref="A2:AI82">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Modif cardinalité slice expertiseType 7c41567fcb14a8abb687abc3b86f688b01a3649a
</commit_message>
<xml_diff>
--- a/lien-specialty-slice-coding/ig/StructureDefinition-ror-practitionerrole.xlsx
+++ b/lien-specialty-slice-coding/ig/StructureDefinition-ror-practitionerrole.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-14T16:30:20+00:00</t>
+    <t>2024-03-15T15:49:47+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -6463,7 +6463,7 @@
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>78</v>
@@ -6579,7 +6579,7 @@
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>87</v>

</xml_diff>

<commit_message>
Correction TRE fixed values a5179b4013e4c734fcc6e57f9d864ce79e7c05f6
</commit_message>
<xml_diff>
--- a/lien-specialty-slice-coding/ig/StructureDefinition-ror-practitionerrole.xlsx
+++ b/lien-specialty-slice-coding/ig/StructureDefinition-ror-practitionerrole.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-19T08:25:58+00:00</t>
+    <t>2024-03-19T09:09:18+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1092,7 +1092,7 @@
   </si>
   <si>
     <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
-  &lt;system value="https://mos.esante.gouv.fr/NOS/JDV_J209-TypeSavoirFaire-ROR/FHIR/JDV-J209-TypeSavoirFaire-ROR"/&gt;
+  &lt;system value="https://mos.esante.gouv.fr/NOS/TRE_R04-TypeSavoirFaire/FHIR/TRE-R04-TypeSavoirFaire"/&gt;
   &lt;code value="S"/&gt;
 &lt;/valueCoding&gt;</t>
   </si>
@@ -1122,7 +1122,7 @@
   </si>
   <si>
     <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
-  &lt;system value="https://mos.esante.gouv.fr/NOS/JDV_J209-TypeSavoirFaire-ROR/FHIR/JDV-J209-TypeSavoirFaire-ROR"/&gt;
+  &lt;system value="https://mos.esante.gouv.fr/NOS/TRE_R04-TypeSavoirFaire/FHIR/TRE-R04-TypeSavoirFaire"/&gt;
   &lt;code value="C"/&gt;
 &lt;/valueCoding&gt;</t>
   </si>
@@ -1152,7 +1152,7 @@
   </si>
   <si>
     <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
-  &lt;system value="https://mos.esante.gouv.fr/NOS/JDV_J209-TypeSavoirFaire-ROR/FHIR/JDV-J209-TypeSavoirFaire-ROR"/&gt;
+  &lt;system value="https://mos.esante.gouv.fr/NOS/TRE_R04-TypeSavoirFaire/FHIR/TRE-R04-TypeSavoirFaire"/&gt;
   &lt;code value="CEX"/&gt;
 &lt;/valueCoding&gt;</t>
   </si>
@@ -1182,7 +1182,7 @@
   </si>
   <si>
     <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
-  &lt;system value="https://mos.esante.gouv.fr/NOS/JDV_J209-TypeSavoirFaire-ROR/FHIR/JDV-J209-TypeSavoirFaire-ROR"/&gt;
+  &lt;system value="https://mos.esante.gouv.fr/NOS/TRE_R04-TypeSavoirFaire/FHIR/TRE-R04-TypeSavoirFaire"/&gt;
   &lt;code value="OP"/&gt;
 &lt;/valueCoding&gt;</t>
   </si>
@@ -1212,7 +1212,7 @@
   </si>
   <si>
     <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
-  &lt;system value="https://mos.esante.gouv.fr/NOS/JDV_J209-TypeSavoirFaire-ROR/FHIR/JDV-J209-TypeSavoirFaire-ROR"/&gt;
+  &lt;system value="https://mos.esante.gouv.fr/NOS/TRE_R04-TypeSavoirFaire/FHIR/TRE-R04-TypeSavoirFaire"/&gt;
   &lt;code value="CAPA"/&gt;
 &lt;/valueCoding&gt;</t>
   </si>
@@ -1242,7 +1242,7 @@
   </si>
   <si>
     <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
-  &lt;system value="https://mos.esante.gouv.fr/NOS/JDV_J209-TypeSavoirFaire-ROR/FHIR/JDV-J209-TypeSavoirFaire-ROR"/&gt;
+  &lt;system value="https://mos.esante.gouv.fr/NOS/TRE_R04-TypeSavoirFaire/FHIR/TRE-R04-TypeSavoirFaire"/&gt;
   &lt;code value="PAC"/&gt;
 &lt;/valueCoding&gt;</t>
   </si>
@@ -1272,7 +1272,7 @@
   </si>
   <si>
     <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
-  &lt;system value="https://mos.esante.gouv.fr/NOS/JDV_J209-TypeSavoirFaire-ROR/FHIR/JDV-J209-TypeSavoirFaire-ROR"/&gt;
+  &lt;system value="https://mos.esante.gouv.fr/NOS/TRE_R04-TypeSavoirFaire/FHIR/TRE-R04-TypeSavoirFaire"/&gt;
   &lt;code value="DNQ"/&gt;
 &lt;/valueCoding&gt;</t>
   </si>
@@ -1302,7 +1302,7 @@
   </si>
   <si>
     <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
-  &lt;system value="https://mos.esante.gouv.fr/NOS/JDV_J209-TypeSavoirFaire-ROR/FHIR/JDV-J209-TypeSavoirFaire-ROR"/&gt;
+  &lt;system value="https://mos.esante.gouv.fr/NOS/TRE_R04-TypeSavoirFaire/FHIR/TRE-R04-TypeSavoirFaire"/&gt;
   &lt;code value="DEC"/&gt;
 &lt;/valueCoding&gt;</t>
   </si>

</xml_diff>

<commit_message>
Modif cardinalités slices coding PR.specialty 96890746d0b7e8a7cfd1134fdd69823eb417e742
</commit_message>
<xml_diff>
--- a/lien-specialty-slice-coding/ig/StructureDefinition-ror-practitionerrole.xlsx
+++ b/lien-specialty-slice-coding/ig/StructureDefinition-ror-practitionerrole.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-19T15:15:55+00:00</t>
+    <t>2024-03-19T16:12:05+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -6765,7 +6765,7 @@
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
-        <v>77</v>
+        <v>196</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>78</v>
@@ -6881,7 +6881,7 @@
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>87</v>
@@ -6999,7 +6999,7 @@
       </c>
       <c r="E43" s="2"/>
       <c r="F43" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>87</v>
@@ -7571,7 +7571,7 @@
       </c>
       <c r="E48" s="2"/>
       <c r="F48" t="s" s="2">
-        <v>77</v>
+        <v>196</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>78</v>
@@ -7687,7 +7687,7 @@
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>87</v>
@@ -7805,7 +7805,7 @@
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G50" t="s" s="2">
         <v>87</v>
@@ -8377,7 +8377,7 @@
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s" s="2">
-        <v>77</v>
+        <v>196</v>
       </c>
       <c r="G55" t="s" s="2">
         <v>78</v>
@@ -8493,7 +8493,7 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G56" t="s" s="2">
         <v>87</v>
@@ -8611,7 +8611,7 @@
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G57" t="s" s="2">
         <v>87</v>
@@ -9181,7 +9181,7 @@
       </c>
       <c r="E62" s="2"/>
       <c r="F62" t="s" s="2">
-        <v>77</v>
+        <v>196</v>
       </c>
       <c r="G62" t="s" s="2">
         <v>78</v>
@@ -9297,7 +9297,7 @@
       </c>
       <c r="E63" s="2"/>
       <c r="F63" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G63" t="s" s="2">
         <v>87</v>
@@ -9415,7 +9415,7 @@
       </c>
       <c r="E64" s="2"/>
       <c r="F64" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G64" t="s" s="2">
         <v>87</v>
@@ -9987,7 +9987,7 @@
       </c>
       <c r="E69" s="2"/>
       <c r="F69" t="s" s="2">
-        <v>77</v>
+        <v>196</v>
       </c>
       <c r="G69" t="s" s="2">
         <v>78</v>
@@ -10103,7 +10103,7 @@
       </c>
       <c r="E70" s="2"/>
       <c r="F70" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G70" t="s" s="2">
         <v>87</v>
@@ -10221,7 +10221,7 @@
       </c>
       <c r="E71" s="2"/>
       <c r="F71" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G71" t="s" s="2">
         <v>87</v>
@@ -10795,7 +10795,7 @@
       </c>
       <c r="E76" s="2"/>
       <c r="F76" t="s" s="2">
-        <v>77</v>
+        <v>196</v>
       </c>
       <c r="G76" t="s" s="2">
         <v>78</v>
@@ -10911,7 +10911,7 @@
       </c>
       <c r="E77" s="2"/>
       <c r="F77" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G77" t="s" s="2">
         <v>87</v>
@@ -11029,7 +11029,7 @@
       </c>
       <c r="E78" s="2"/>
       <c r="F78" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G78" t="s" s="2">
         <v>87</v>
@@ -11601,7 +11601,7 @@
       </c>
       <c r="E83" s="2"/>
       <c r="F83" t="s" s="2">
-        <v>77</v>
+        <v>196</v>
       </c>
       <c r="G83" t="s" s="2">
         <v>78</v>
@@ -11717,7 +11717,7 @@
       </c>
       <c r="E84" s="2"/>
       <c r="F84" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G84" t="s" s="2">
         <v>87</v>
@@ -11835,7 +11835,7 @@
       </c>
       <c r="E85" s="2"/>
       <c r="F85" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G85" t="s" s="2">
         <v>87</v>
@@ -12407,7 +12407,7 @@
       </c>
       <c r="E90" s="2"/>
       <c r="F90" t="s" s="2">
-        <v>77</v>
+        <v>196</v>
       </c>
       <c r="G90" t="s" s="2">
         <v>78</v>
@@ -12523,7 +12523,7 @@
       </c>
       <c r="E91" s="2"/>
       <c r="F91" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G91" t="s" s="2">
         <v>87</v>
@@ -12641,7 +12641,7 @@
       </c>
       <c r="E92" s="2"/>
       <c r="F92" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G92" t="s" s="2">
         <v>87</v>

</xml_diff>